<commit_message>
Lux MeasureMent Sensor Calib
</commit_message>
<xml_diff>
--- a/Final_Project/raw_data_calib.xlsx
+++ b/Final_Project/raw_data_calib.xlsx
@@ -5,23 +5,24 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Google Drive\UC\2018-2019\1º Semestre\Sensores Inteligentes\SI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Google Drive\UC\2018-2019\1º Semestre\Sensores Inteligentes\SI_Repo_ESM\Final_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D6C03AA-1CE2-481B-97E6-E9BDD46AC2DF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1473D8D3-93E8-47C5-8D7A-20B05C694B05}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7560" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Luz Max" sheetId="1" r:id="rId1"/>
     <sheet name="Luz Min" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="25">
   <si>
     <t>A</t>
   </si>
@@ -62,9 +63,6 @@
     <t>Lux</t>
   </si>
   <si>
-    <t>Adc Values (Min/Max)</t>
-  </si>
-  <si>
     <t>LDR's</t>
   </si>
   <si>
@@ -93,6 +91,12 @@
   </si>
   <si>
     <t>RD</t>
+  </si>
+  <si>
+    <t>ADC Values (Min/Max)</t>
+  </si>
+  <si>
+    <t>Resistance Values (Min/Max)</t>
   </si>
 </sst>
 </file>
@@ -243,7 +247,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="39">
+  <fills count="41">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -455,12 +459,24 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.249977111117893"/>
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="24">
+  <borders count="42">
     <border>
       <left/>
       <right/>
@@ -745,8 +761,244 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -789,11 +1041,10 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="35" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -834,11 +1085,99 @@
     <xf numFmtId="0" fontId="0" fillId="36" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="35" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="35" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="35" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="35" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="35" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="35" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="38" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="35" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="35" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="35" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="35" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="37" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -846,14 +1185,27 @@
     <xf numFmtId="0" fontId="16" fillId="37" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="39" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="39" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="40" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="40" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="42" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -893,6 +1245,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Percent" xfId="42" builtinId="5"/>
     <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
@@ -924,6 +1277,73 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:effectLst>
+                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                    <a:prstClr val="black">
+                      <a:alpha val="40000"/>
+                    </a:prstClr>
+                  </a:outerShdw>
+                </a:effectLst>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>LDR's ADC Values/Lux</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -1010,8 +1430,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="0.1449074475462177"/>
-                  <c:y val="0.41308687160373608"/>
+                  <c:x val="0.14490880327728389"/>
+                  <c:y val="0.29308395644499097"/>
                 </c:manualLayout>
               </c:layout>
               <c:tx>
@@ -1184,8 +1604,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="0.15509706454086281"/>
-                  <c:y val="0.60209436507003788"/>
+                  <c:x val="0.15543744172486071"/>
+                  <c:y val="0.43474245820028162"/>
                 </c:manualLayout>
               </c:layout>
               <c:tx>
@@ -1358,8 +1778,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="0.15705281559623688"/>
-                  <c:y val="0.49902500993345983"/>
+                  <c:x val="0.15062251560554205"/>
+                  <c:y val="0.33760897016336427"/>
                 </c:manualLayout>
               </c:layout>
               <c:tx>
@@ -1532,8 +1952,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="0.15705281559623688"/>
-                  <c:y val="0.46469318200896531"/>
+                  <c:x val="0.16185734321728562"/>
+                  <c:y val="0.29366045868951518"/>
                 </c:manualLayout>
               </c:layout>
               <c:tx>
@@ -1658,6 +2078,59 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>LUX</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1717,6 +2190,59 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>adc VALUE</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1848,7 +2374,1649 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:effectLst>
+                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                    <a:prstClr val="black">
+                      <a:alpha val="40000"/>
+                    </a:prstClr>
+                  </a:outerShdw>
+                </a:effectLst>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>LDR</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t>'s Resistance/Lux</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.11619498326715952"/>
+          <c:y val="4.1918575895727096E-2"/>
+          <c:w val="0.83825889335989201"/>
+          <c:h val="0.69627629125544821"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>LDR_A</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent1">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent1">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent1">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDash"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="exp"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="9.2047110410010291E-2"/>
+                  <c:y val="-0.24809906494408657"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1">
+                          <a:lumMod val="75000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Luz Max'!$F$31:$F$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Luz Max'!$G$31:$G$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>320770.90163934423</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6061.5384615384628</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-5D54-4562-91A3-BE825C38E0F8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>LDR_B</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent2">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent2">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDash"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="exp"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="8.9783386584317115E-2"/>
+                  <c:y val="-0.31581368754487649"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1">
+                          <a:lumMod val="75000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Luz Max'!$F$31:$F$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Luz Max'!$H$31:$H$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>219664.40340909094</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>323.44262295082081</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-5D54-4562-91A3-BE825C38E0F8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>LDR_C</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="9525" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent3">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent3">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent3">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+                <a:prstDash val="sysDash"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="exp"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="7.2114933001795833E-2"/>
+                  <c:y val="-0.38030380430753363"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1">
+                          <a:lumMod val="75000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Luz Max'!$F$31:$F$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Luz Max'!$I$31:$I$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>13387660.000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1086.1187957689199</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-5D54-4562-91A3-BE825C38E0F8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>LDR_D</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent4">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent4">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent4">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+                <a:prstDash val="sysDash"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="exp"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="6.7587485350409301E-2"/>
+                  <c:y val="-0.4480184269083235"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1">
+                          <a:lumMod val="75000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Luz Max'!$F$31:$F$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Luz Max'!$J$31:$J$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>2675119.9999999995</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>590.66010872379229</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-5D54-4562-91A3-BE825C38E0F8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="67996287"/>
+        <c:axId val="337473407"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="67996287"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>lUX</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="337473407"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="337473407"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>RESISTANCE</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> </a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="67996287"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>A</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:glow rad="139700">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="14000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:glow rad="63500">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="175000"/>
+                    <a:alpha val="25000"/>
+                  </a:schemeClr>
+                </a:glow>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="25400" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1">
+                    <a:alpha val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="log"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="4.0797900262467192E-2"/>
+                  <c:y val="-6.0941236512102655E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1">
+                          <a:lumMod val="75000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$5:$C$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>400</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$5:$D$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.45500000000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.33</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.75</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-743A-405E-A5DD-4AA345E138A4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>B</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:glow rad="139700">
+                <a:schemeClr val="accent2">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="14000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:glow rad="63500">
+                  <a:schemeClr val="accent2">
+                    <a:satMod val="175000"/>
+                    <a:alpha val="25000"/>
+                  </a:schemeClr>
+                </a:glow>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="25400" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2">
+                    <a:alpha val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="log"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="2.5631233595800523E-2"/>
+                  <c:y val="6.2868547681539808E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1">
+                          <a:lumMod val="75000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$5:$C$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>400</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$5:$E$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>4.55</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.67</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.25</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-743A-405E-A5DD-4AA345E138A4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1599122992"/>
+        <c:axId val="1697161792"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1599122992"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                  <a:alpha val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1697161792"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1697161792"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                  <a:alpha val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1599122992"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -2390,20 +4558,1060 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="248">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="245">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="15000"/>
+        <a:lumOff val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="139700">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="14000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:lumMod val="60000"/>
+          <a:lumOff val="40000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="3"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="50000"/>
+          <a:lumOff val="50000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+            <a:alpha val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="1" kern="1200" cap="none" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>269081</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:colOff>11906</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2411,6 +5619,83 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6FAB1F41-DA6C-43CB-A0DE-701B35C2BB82}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>171449</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A4692F7F-B6A1-444B-B4D8-2A9AD1E8FF2B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>185736</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>38099</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F365835D-D634-4631-9EF1-D98840048F19}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2730,8 +6015,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U118"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="W22" sqref="W22"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AA10" sqref="AA10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2796,7 +6081,7 @@
         <v>3795</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2402</v>
       </c>
@@ -2809,14 +6094,13 @@
       <c r="D5">
         <v>3782</v>
       </c>
-      <c r="G5" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="H5" s="21"/>
-      <c r="I5" s="21"/>
-      <c r="J5" s="21"/>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="F5" s="47"/>
+      <c r="G5" s="48"/>
+      <c r="H5" s="48"/>
+      <c r="I5" s="48"/>
+      <c r="J5" s="48"/>
+    </row>
+    <row r="6" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2488</v>
       </c>
@@ -2829,20 +6113,23 @@
       <c r="D6">
         <v>3823</v>
       </c>
-      <c r="G6" s="17" t="s">
+      <c r="F6" s="57" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="H6" s="17" t="s">
+      <c r="H6" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="I6" s="17" t="s">
+      <c r="I6" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="J6" s="17" t="s">
+      <c r="J6" s="36" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2455</v>
       </c>
@@ -2855,13 +6142,13 @@
       <c r="D7">
         <v>3815</v>
       </c>
-      <c r="F7" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="G7" s="22"/>
-      <c r="H7" s="22"/>
-      <c r="I7" s="22"/>
-      <c r="J7" s="22"/>
+      <c r="F7" s="58"/>
+      <c r="G7" s="53" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" s="53"/>
+      <c r="I7" s="53"/>
+      <c r="J7" s="54"/>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -2876,26 +6163,26 @@
       <c r="D8">
         <v>3859</v>
       </c>
-      <c r="F8" s="18" t="s">
+      <c r="F8" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="40">
         <f>AVERAGE(A:A)</f>
         <v>2475.8050847457625</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="33">
         <f>AVERAGE(B:B)</f>
         <v>3943.2372881355932</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="33">
         <f>AVERAGE(C:C)</f>
         <v>3646.398305084746</v>
       </c>
-      <c r="J8">
+      <c r="J8" s="34">
         <f>AVERAGE(D:D)</f>
         <v>3820.6864406779659</v>
       </c>
-      <c r="U8" s="3"/>
+      <c r="U8" s="1"/>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9">
@@ -2910,27 +6197,27 @@
       <c r="D9">
         <v>3855</v>
       </c>
-      <c r="F9" s="18" t="s">
+      <c r="F9" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="41">
         <f>MIN(A:A)</f>
         <v>2402</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="27">
         <f>MIN(B:B)</f>
         <v>3904</v>
       </c>
-      <c r="I9">
+      <c r="I9" s="27">
         <f>MIN(C:C)</f>
         <v>3584</v>
       </c>
-      <c r="J9">
+      <c r="J9" s="29">
         <f>MIN(D:D)</f>
         <v>3760</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>2501</v>
       </c>
@@ -2943,27 +6230,27 @@
       <c r="D10">
         <v>3847</v>
       </c>
-      <c r="F10" s="18" t="s">
+      <c r="F10" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="G10" s="1">
+      <c r="G10" s="42">
         <f>MAX(A:A)</f>
         <v>2535</v>
       </c>
-      <c r="H10" s="1">
+      <c r="H10" s="37">
         <f>MAX(B:B)</f>
         <v>3965</v>
       </c>
-      <c r="I10" s="1">
+      <c r="I10" s="37">
         <f>MAX(C:C)</f>
         <v>3687</v>
       </c>
-      <c r="J10" s="1">
+      <c r="J10" s="38">
         <f>MAX(D:D)</f>
         <v>3863</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>2514</v>
       </c>
@@ -2976,7 +6263,13 @@
       <c r="D11">
         <v>3851</v>
       </c>
-      <c r="F11" s="18"/>
+      <c r="F11" s="39"/>
+      <c r="G11" s="55" t="s">
+        <v>14</v>
+      </c>
+      <c r="H11" s="55"/>
+      <c r="I11" s="55"/>
+      <c r="J11" s="56"/>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12">
@@ -2991,13 +6284,25 @@
       <c r="D12">
         <v>3799</v>
       </c>
-      <c r="F12" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="G12" s="22"/>
-      <c r="H12" s="22"/>
-      <c r="I12" s="22"/>
-      <c r="J12" s="22"/>
+      <c r="F12" s="45" t="s">
+        <v>4</v>
+      </c>
+      <c r="G12" s="40">
+        <f>AVERAGE('Luz Min'!A:A)</f>
+        <v>144.14285714285714</v>
+      </c>
+      <c r="H12" s="33">
+        <f>AVERAGE('Luz Min'!B:B)</f>
+        <v>210.9047619047619</v>
+      </c>
+      <c r="I12" s="33">
+        <f>AVERAGE('Luz Min'!C:C)</f>
+        <v>11</v>
+      </c>
+      <c r="J12" s="34">
+        <f>AVERAGE('Luz Min'!D:D)</f>
+        <v>23.404761904761905</v>
+      </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13">
@@ -3012,27 +6317,27 @@
       <c r="D13">
         <v>3815</v>
       </c>
-      <c r="F13" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="G13">
-        <f>AVERAGE('Luz Min'!A:A)</f>
-        <v>144.14285714285714</v>
-      </c>
-      <c r="H13">
-        <f>AVERAGE('Luz Min'!B:B)</f>
-        <v>210.9047619047619</v>
-      </c>
-      <c r="I13">
-        <f>AVERAGE('Luz Min'!C:C)</f>
-        <v>11</v>
-      </c>
-      <c r="J13">
-        <f>AVERAGE('Luz Min'!D:D)</f>
-        <v>23.404761904761905</v>
-      </c>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="F13" s="45" t="s">
+        <v>5</v>
+      </c>
+      <c r="G13" s="43">
+        <f>MIN('Luz Min'!A:A)</f>
+        <v>122</v>
+      </c>
+      <c r="H13" s="28">
+        <f>MIN('Luz Min'!B:B)</f>
+        <v>176</v>
+      </c>
+      <c r="I13" s="28">
+        <f>MIN('Luz Min'!C:C)</f>
+        <v>3</v>
+      </c>
+      <c r="J13" s="30">
+        <f>MIN('Luz Min'!D:D)</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>2444</v>
       </c>
@@ -3045,24 +6350,24 @@
       <c r="D14">
         <v>3798</v>
       </c>
-      <c r="F14" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="G14" s="2">
-        <f>MIN('Luz Min'!A:A)</f>
-        <v>122</v>
-      </c>
-      <c r="H14" s="2">
-        <f>MIN('Luz Min'!B:B)</f>
-        <v>176</v>
-      </c>
-      <c r="I14" s="2">
-        <f>MIN('Luz Min'!C:C)</f>
-        <v>3</v>
-      </c>
-      <c r="J14" s="2">
-        <f>MIN('Luz Min'!D:D)</f>
-        <v>15</v>
+      <c r="F14" s="46" t="s">
+        <v>6</v>
+      </c>
+      <c r="G14" s="44">
+        <f>MAX('Luz Min'!A:A)</f>
+        <v>155</v>
+      </c>
+      <c r="H14" s="31">
+        <f>MAX('Luz Min'!B:B)</f>
+        <v>220</v>
+      </c>
+      <c r="I14" s="31">
+        <f>MAX('Luz Min'!C:C)</f>
+        <v>17</v>
+      </c>
+      <c r="J14" s="32">
+        <f>MAX('Luz Min'!D:D)</f>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
@@ -3078,25 +6383,6 @@
       <c r="D15">
         <v>3784</v>
       </c>
-      <c r="F15" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="G15">
-        <f>MAX('Luz Min'!A:A)</f>
-        <v>155</v>
-      </c>
-      <c r="H15">
-        <f>MAX('Luz Min'!B:B)</f>
-        <v>220</v>
-      </c>
-      <c r="I15">
-        <f>MAX('Luz Min'!C:C)</f>
-        <v>17</v>
-      </c>
-      <c r="J15">
-        <f>MAX('Luz Min'!D:D)</f>
-        <v>28</v>
-      </c>
     </row>
     <row r="16" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16">
@@ -3125,15 +6411,15 @@
       <c r="D17">
         <v>3830</v>
       </c>
-      <c r="F17" s="13" t="s">
+      <c r="F17" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="G17" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="H17" s="19"/>
-      <c r="I17" s="19"/>
-      <c r="J17" s="20"/>
+      <c r="G17" s="51" t="s">
+        <v>23</v>
+      </c>
+      <c r="H17" s="51"/>
+      <c r="I17" s="51"/>
+      <c r="J17" s="52"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18">
@@ -3148,19 +6434,19 @@
       <c r="D18">
         <v>3858</v>
       </c>
-      <c r="F18" s="6" t="s">
+      <c r="F18" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G18" s="4" t="s">
+      <c r="G18" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H18" s="14" t="s">
+      <c r="H18" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="I18" s="14" t="s">
+      <c r="I18" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="J18" s="5" t="s">
+      <c r="J18" s="3" t="s">
         <v>11</v>
       </c>
     </row>
@@ -3177,23 +6463,23 @@
       <c r="D19">
         <v>3863</v>
       </c>
-      <c r="F19" s="7">
+      <c r="F19" s="5">
         <v>5</v>
       </c>
-      <c r="G19" s="8">
-        <f>G14</f>
+      <c r="G19" s="6">
+        <f>G13</f>
         <v>122</v>
       </c>
-      <c r="H19" s="15">
-        <f>H14</f>
+      <c r="H19" s="13">
+        <f>H13</f>
         <v>176</v>
       </c>
-      <c r="I19" s="15">
-        <f>I14</f>
+      <c r="I19" s="13">
+        <f>I13</f>
         <v>3</v>
       </c>
-      <c r="J19" s="9">
-        <f>J14</f>
+      <c r="J19" s="7">
+        <f>J13</f>
         <v>15</v>
       </c>
     </row>
@@ -3210,22 +6496,22 @@
       <c r="D20">
         <v>3831</v>
       </c>
-      <c r="F20" s="10">
+      <c r="F20" s="8">
         <v>1000</v>
       </c>
-      <c r="G20" s="11">
+      <c r="G20" s="9">
         <f>G10</f>
         <v>2535</v>
       </c>
-      <c r="H20" s="16">
+      <c r="H20" s="14">
         <f>H10</f>
         <v>3965</v>
       </c>
-      <c r="I20" s="16">
+      <c r="I20" s="14">
         <f>I10</f>
         <v>3687</v>
       </c>
-      <c r="J20" s="12">
+      <c r="J20" s="10">
         <f>J10</f>
         <v>3863</v>
       </c>
@@ -3272,13 +6558,13 @@
         <v>3797</v>
       </c>
       <c r="F23" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G23">
         <v>4.7</v>
       </c>
       <c r="I23" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J23">
         <f>9.85*10^3</f>
@@ -3299,13 +6585,13 @@
         <v>3815</v>
       </c>
       <c r="F24" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G24">
         <v>12</v>
       </c>
       <c r="I24" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J24">
         <v>9865</v>
@@ -3325,14 +6611,14 @@
         <v>3799</v>
       </c>
       <c r="F25" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G25">
         <f>G23/((2^G24)-1)</f>
         <v>1.1477411477411477E-3</v>
       </c>
       <c r="I25" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J25">
         <v>9815</v>
@@ -3352,7 +6638,7 @@
         <v>3857</v>
       </c>
       <c r="I26" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J26">
         <v>9835</v>
@@ -3372,7 +6658,7 @@
         <v>3843</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>2513</v>
       </c>
@@ -3386,7 +6672,7 @@
         <v>3853</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>2520</v>
       </c>
@@ -3399,8 +6685,17 @@
       <c r="D29">
         <v>3856</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F29" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G29" s="51" t="s">
+        <v>24</v>
+      </c>
+      <c r="H29" s="51"/>
+      <c r="I29" s="51"/>
+      <c r="J29" s="52"/>
+    </row>
+    <row r="30" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>2451</v>
       </c>
@@ -3412,6 +6707,21 @@
       </c>
       <c r="D30">
         <v>3809</v>
+      </c>
+      <c r="F30" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="G30" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="H30" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="I30" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="J30" s="18" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
@@ -3427,8 +6737,27 @@
       <c r="D31">
         <v>3827</v>
       </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F31" s="19">
+        <v>5</v>
+      </c>
+      <c r="G31" s="20">
+        <f>($J$23/(G13*$G$25))*$G$23-$J$23</f>
+        <v>320770.90163934423</v>
+      </c>
+      <c r="H31" s="21">
+        <f>($J$24/(H13*$G$25))*$G$23-$J$24</f>
+        <v>219664.40340909094</v>
+      </c>
+      <c r="I31" s="21">
+        <f>($J$25/(I13*$G$25))*$G$23-$J$25</f>
+        <v>13387660.000000002</v>
+      </c>
+      <c r="J31" s="22">
+        <f>($J$26/(J13*$G$25))*$G$23-$J$26</f>
+        <v>2675119.9999999995</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>2428</v>
       </c>
@@ -3440,6 +6769,25 @@
       </c>
       <c r="D32">
         <v>3791</v>
+      </c>
+      <c r="F32" s="23">
+        <v>1000</v>
+      </c>
+      <c r="G32" s="24">
+        <f>($J23/(G10*$G$25))*$G$23-$J23</f>
+        <v>6061.5384615384628</v>
+      </c>
+      <c r="H32" s="25">
+        <f>($J$24/(H10*$G$25))*$G$23-$J$24</f>
+        <v>323.44262295082081</v>
+      </c>
+      <c r="I32" s="25">
+        <f>($J$25/(I10*$G$25))*$G$23-$J$25</f>
+        <v>1086.1187957689199</v>
+      </c>
+      <c r="J32" s="26">
+        <f>($J$26/(J10*$G$25))*$G$23-$J$26</f>
+        <v>590.66010872379229</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -4647,11 +7995,12 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="G17:J17"/>
-    <mergeCell ref="G5:J5"/>
-    <mergeCell ref="F7:J7"/>
-    <mergeCell ref="F12:J12"/>
+    <mergeCell ref="G29:J29"/>
+    <mergeCell ref="G7:J7"/>
+    <mergeCell ref="G11:J11"/>
+    <mergeCell ref="F6:F7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5260,4 +8609,114 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{607371D4-D577-4CFD-A295-1888B179722B}">
+  <dimension ref="B2:E9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="V18" sqref="V18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B2">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="59">
+        <v>0.01</v>
+      </c>
+      <c r="C5">
+        <f>$B$2*B5</f>
+        <v>10</v>
+      </c>
+      <c r="D5">
+        <f>455*10^-3</f>
+        <v>0.45500000000000002</v>
+      </c>
+      <c r="E5">
+        <v>4.55</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="59">
+        <v>0.1</v>
+      </c>
+      <c r="C6">
+        <f t="shared" ref="C6:C9" si="0">$B$2*B6</f>
+        <v>100</v>
+      </c>
+      <c r="D6">
+        <v>2.5</v>
+      </c>
+      <c r="E6">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="59">
+        <v>0.2</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>200</v>
+      </c>
+      <c r="D7">
+        <v>3.33</v>
+      </c>
+      <c r="E7">
+        <v>1.67</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="59">
+        <v>0.3</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>300</v>
+      </c>
+      <c r="D8">
+        <v>3.75</v>
+      </c>
+      <c r="E8">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B9" s="59">
+        <v>0.4</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>400</v>
+      </c>
+      <c r="D9">
+        <v>4</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>